<commit_message>
actualizacion de cronograma de desarrollo
</commit_message>
<xml_diff>
--- a/resumen/cronograma de actividades desarrollo web mateo.xlsx
+++ b/resumen/cronograma de actividades desarrollo web mateo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\Documentos\pagina web mateo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\mateo2\resumen\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
   <si>
     <t>Item</t>
   </si>
@@ -276,6 +276,65 @@
   </si>
   <si>
     <t>Actualización de repositorio en la nube implementando git hub, carga de archivos al repositorio remoto en la nuve, creacion de copia local.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Actualización de plantilla administrativa y sincronizacion con los controladores de enrutamiento para el modulo </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>multimedia</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Creacion de controladores del </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">CRUD (CREAR CONSULTAR ELIMINAR) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">para el modulo </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>multimedia</t>
+    </r>
+  </si>
+  <si>
+    <t>Dento de esta creacion de controladores se crearon sus respectivos modelos y formularios, se configuraron los archivos js que hacen el respectivo redireccionamiento al controlador correspondiente. para la creacion de elementos multimedia, ya se creaN los elementos DESDE FORMULARIOS ESTABLECIDOS CON SUS RESPECTIVAS VALIDACIONES y son sincronizados con la vista que muestra los archivos dentro del panel de administración</t>
+  </si>
+  <si>
+    <t>Pendiente para cambiar colores</t>
   </si>
 </sst>
 </file>
@@ -337,7 +396,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -360,11 +419,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -375,14 +445,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -665,31 +744,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:H16"/>
+  <dimension ref="B2:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="5.5703125" customWidth="1"/>
-    <col min="3" max="3" width="31.5703125" customWidth="1"/>
-    <col min="4" max="4" width="54.140625" customWidth="1"/>
+    <col min="1" max="1" width="5.28515625" customWidth="1"/>
+    <col min="2" max="2" width="5.5703125" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="34.5703125" customWidth="1"/>
+    <col min="4" max="4" width="66.85546875" customWidth="1"/>
     <col min="5" max="5" width="21.7109375" customWidth="1"/>
     <col min="6" max="6" width="20.28515625" customWidth="1"/>
     <col min="8" max="8" width="33.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
     </row>
     <row r="3" spans="3:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C3" s="3" t="s">
@@ -844,10 +924,10 @@
       </c>
     </row>
     <row r="11" spans="3:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="8" t="s">
         <v>25</v>
       </c>
       <c r="E11" s="2">
@@ -859,13 +939,13 @@
       <c r="G11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="5"/>
+      <c r="H11" s="4"/>
     </row>
     <row r="12" spans="3:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="7"/>
+      <c r="D12" s="8"/>
       <c r="E12" s="2">
         <v>44100</v>
       </c>
@@ -875,13 +955,13 @@
       <c r="G12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H12" s="5"/>
+      <c r="H12" s="4"/>
     </row>
     <row r="13" spans="3:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="7"/>
+      <c r="D13" s="8"/>
       <c r="E13" s="2">
         <v>44100</v>
       </c>
@@ -891,13 +971,13 @@
       <c r="G13" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H13" s="5"/>
+      <c r="H13" s="4"/>
     </row>
     <row r="14" spans="3:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="7"/>
+      <c r="D14" s="8"/>
       <c r="E14" s="2">
         <v>44100</v>
       </c>
@@ -907,13 +987,13 @@
       <c r="G14" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H14" s="5"/>
+      <c r="H14" s="4"/>
     </row>
     <row r="15" spans="3:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="7"/>
+      <c r="D15" s="8"/>
       <c r="E15" s="2">
         <v>44100</v>
       </c>
@@ -923,13 +1003,13 @@
       <c r="G15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H15" s="5"/>
+      <c r="H15" s="4"/>
     </row>
     <row r="16" spans="3:8" ht="75" x14ac:dyDescent="0.25">
       <c r="C16" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="5"/>
+      <c r="D16" s="4"/>
       <c r="E16" s="2">
         <v>44100</v>
       </c>
@@ -939,7 +1019,35 @@
       <c r="G16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H16" s="5"/>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="3:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="C17" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="3:8" ht="114" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="2">
+        <v>44102</v>
+      </c>
+      <c r="F18" s="2">
+        <v>44102</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>